<commit_message>
Finalizing the task and adding verify order details test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/AutomationPractice.xlsx
+++ b/src/test/resources/TestDataFiles/AutomationPractice.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Variable</t>
   </si>
@@ -96,49 +96,46 @@
     <t>address alias</t>
   </si>
   <si>
+    <t>magdy</t>
+  </si>
+  <si>
+    <t>heiba</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>111-222-3333</t>
+  </si>
+  <si>
+    <t>333-222-1111</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>mr</t>
   </si>
   <si>
-    <t>magdy</t>
-  </si>
-  <si>
-    <t>heiba</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>first name</t>
-  </si>
-  <si>
-    <t>last name</t>
-  </si>
-  <si>
-    <t>Address 2</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>111-222-3333</t>
-  </si>
-  <si>
-    <t>333-222-1111</t>
-  </si>
-  <si>
-    <t>12345678</t>
-  </si>
-  <si>
-    <t>mh3@mail.com</t>
-  </si>
-  <si>
-    <t>11</t>
+    <t>mj@mail.com</t>
   </si>
 </sst>
 </file>
@@ -532,7 +529,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,7 +2601,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2612,7 +2609,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2620,7 +2617,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2636,7 +2633,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2652,7 +2649,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2668,7 +2665,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2676,7 +2673,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2684,7 +2681,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2692,7 +2689,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
@@ -2716,7 +2713,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2724,7 +2721,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2732,7 +2729,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2748,7 +2745,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2764,7 +2761,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2772,7 +2769,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>